<commit_message>
final update excel / app finished - v.4.1
</commit_message>
<xml_diff>
--- a/Incidencias_Pideu.xlsx
+++ b/Incidencias_Pideu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\APP_INCIDENTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D807386-C650-4880-87B0-7D1727807C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DCCE8BB-E236-4F19-9D95-C0B4FB6656FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,9 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
-  <si>
-    <t>Fecha y Hora</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Hora</t>
   </si>
   <si>
     <t>WC47 NACP</t>
@@ -40,52 +43,31 @@
     <t>SPL</t>
   </si>
   <si>
-    <t>2024-05-10 11:43:16</t>
-  </si>
-  <si>
-    <t>No atornilla tapa</t>
-  </si>
-  <si>
-    <t>2024-05-10 11:43:18</t>
-  </si>
-  <si>
-    <t>AOI no detecta pieza</t>
-  </si>
-  <si>
-    <t>2024-05-10 11:43:20</t>
-  </si>
-  <si>
-    <t>Cámara no detecta foam derecho</t>
-  </si>
-  <si>
-    <t>2024-05-10 11:43:21</t>
-  </si>
-  <si>
-    <t>Detección de sealling mal puesto</t>
-  </si>
-  <si>
-    <t>2024-05-10 11:43:23</t>
-  </si>
-  <si>
-    <t>NOK Soldad. Plástico+Metal</t>
-  </si>
-  <si>
-    <t>2024-05-10 11:43:26</t>
-  </si>
-  <si>
-    <t>Fallo dispensación glue</t>
-  </si>
-  <si>
-    <t>2024-05-10 11:44:00</t>
-  </si>
-  <si>
-    <t>Cámara no detecta skeleton</t>
-  </si>
-  <si>
-    <t>2024-05-10 11:44:18</t>
-  </si>
-  <si>
-    <t>Sensor de PCB detecta que hay placa cuando no la hay</t>
+    <t>2024-05-10</t>
+  </si>
+  <si>
+    <t>11:54:47</t>
+  </si>
+  <si>
+    <t>Palet atascado en la curva</t>
+  </si>
+  <si>
+    <t>11:54:49</t>
+  </si>
+  <si>
+    <t>QR desplazado</t>
+  </si>
+  <si>
+    <t>11:54:51</t>
+  </si>
+  <si>
+    <t>Error en sensor de salida</t>
+  </si>
+  <si>
+    <t>11:54:54</t>
+  </si>
+  <si>
+    <t>Fallo etiqueta</t>
   </si>
 </sst>
 </file>
@@ -124,17 +106,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
+      <left style="thin">
+        <color auto="1"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
+      <right style="thin">
+        <color auto="1"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
+      <top style="thin">
+        <color auto="1"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -449,23 +431,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="C8" sqref="C7:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" customWidth="1"/>
-    <col min="3" max="3" width="32.28515625" customWidth="1"/>
-    <col min="4" max="4" width="35.7109375" customWidth="1"/>
-    <col min="5" max="5" width="27.85546875" customWidth="1"/>
-    <col min="6" max="6" width="49.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+    <col min="6" max="6" width="33.140625" customWidth="1"/>
+    <col min="7" max="7" width="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -484,69 +467,52 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new window - testing.py / v.5.0
</commit_message>
<xml_diff>
--- a/Incidencias_Pideu.xlsx
+++ b/Incidencias_Pideu.xlsx
@@ -1,103 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\APP_INCIDENTS\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DCCE8BB-E236-4F19-9D95-C0B4FB6656FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Incidencias" sheetId="1" r:id="rId1"/>
+    <sheet name="Incidencias" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
-  <si>
-    <t>Fecha</t>
-  </si>
-  <si>
-    <t>Hora</t>
-  </si>
-  <si>
-    <t>WC47 NACP</t>
-  </si>
-  <si>
-    <t>WC48 POWER 5F</t>
-  </si>
-  <si>
-    <t>WC49 POWER 5H</t>
-  </si>
-  <si>
-    <t>WV50 FILTER</t>
-  </si>
-  <si>
-    <t>SPL</t>
-  </si>
-  <si>
-    <t>2024-05-10</t>
-  </si>
-  <si>
-    <t>11:54:47</t>
-  </si>
-  <si>
-    <t>Palet atascado en la curva</t>
-  </si>
-  <si>
-    <t>11:54:49</t>
-  </si>
-  <si>
-    <t>QR desplazado</t>
-  </si>
-  <si>
-    <t>11:54:51</t>
-  </si>
-  <si>
-    <t>Error en sensor de salida</t>
-  </si>
-  <si>
-    <t>11:54:54</t>
-  </si>
-  <si>
-    <t>Fallo etiqueta</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -105,44 +42,85 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -430,93 +408,286 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C7:C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
-    <col min="6" max="6" width="33.140625" customWidth="1"/>
-    <col min="7" max="7" width="38" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Fecha</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Hora</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>WC48 POWER 5F</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>WC49 POWER 5H</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>SPL</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2024-05-10</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>12:30:18</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>No atornilla tapa</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2024-05-10</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>12:30:21</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Cámara no detecta skeleton</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2024-05-10</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>12:30:22</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Detección de sealling mal puesto</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2024-05-10</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>12:30:24</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>No coloca bien la pcb</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2024-05-10</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>12:33:47</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Fallo tolva</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2024-05-10</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>12:50:17</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>No atornilla tapa</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2024-05-10</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>12:50:18</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Tornillo atascado</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2024-05-10</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>12:52:54</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>WC47 NACP</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>No coge placa</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2024-05-10</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>12:53:00</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>WC48 POWER 5F</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>AOI (malla)</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2024-05-10</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>12:53:05</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>WC49 POWER 5H</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Power atascado en prensa, cuesta sacar</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2024-05-10</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>12:53:10</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>WV50 FILTER</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Core enganchado</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024-05-10</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>12:53:13</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>SPL</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Marco atascado en parte inferior</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
perfect excel update and ticket confirms - testing v.5
</commit_message>
<xml_diff>
--- a/Incidencias_Pideu.xlsx
+++ b/Incidencias_Pideu.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
@@ -651,15 +651,134 @@
           <t>10:43:58</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr">
         <is>
           <t>Power atascado en prensa, cuesta sacar</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>10:47:02</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Palet atascado en la curva</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>10:47:05</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Etiquetadora</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>10:47:07</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>QR desplazado</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>10:47:11</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Soldadura defectuosa</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>10:47:14</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>No coloca bien el sealling</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>10:47:17</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Atasco tuerca</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2024-05-13</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>10:47:56</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>No coloca bien el sealling</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>